<commit_message>
feat: Add month and hour column
</commit_message>
<xml_diff>
--- a/POE_2023.xlsx
+++ b/POE_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ottoc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ottoc\Documents\galileo\maestría\2dotrimestre\statisticalLearning\lab1_19001395_V_EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47089C1-8A7D-4484-9557-3EA858679DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D711D923-5E6D-4F70-A17D-82DE6AC61974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8E34DE49-2EF7-4365-BA2D-B79A08C1FB26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="8" xr2:uid="{8E34DE49-2EF7-4365-BA2D-B79A08C1FB26}"/>
   </bookViews>
   <sheets>
     <sheet name="ENERO" sheetId="2" r:id="rId1"/>
@@ -304,47 +304,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
   <si>
     <t xml:space="preserve"> 24:00</t>
   </si>
   <si>
-    <t>Hora</t>
+    <t>horaInicio</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>HoraFin</t>
   </si>
   <si>
-    <t>Enero</t>
-  </si>
-  <si>
-    <t>Febrero</t>
-  </si>
-  <si>
-    <t>Marzo</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Mayo</t>
-  </si>
-  <si>
-    <t>Junio</t>
-  </si>
-  <si>
-    <t>Agosto</t>
+    <t xml:space="preserve"> 24:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +357,12 @@
       <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -499,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -533,13 +522,15 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1757,13 +1748,14 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.08984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.08984375" style="1" customWidth="1"/>
@@ -1780,10 +1772,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -1877,34 +1871,20 @@
       <c r="AG1" s="12">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
       <c r="AO1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="18">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="C2" s="8">
@@ -2010,10 +1990,10 @@
       <c r="AO2" s="2"/>
     </row>
     <row r="3" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="17">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="18">
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="C3" s="8">
@@ -2119,10 +2099,10 @@
       <c r="AO3" s="2"/>
     </row>
     <row r="4" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="18">
         <v>0.125</v>
       </c>
       <c r="C4" s="8">
@@ -2228,10 +2208,10 @@
       <c r="AO4" s="2"/>
     </row>
     <row r="5" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="17">
         <v>0.125</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="18">
         <v>0.16666666666666699</v>
       </c>
       <c r="C5" s="8">
@@ -2337,10 +2317,10 @@
       <c r="AO5" s="2"/>
     </row>
     <row r="6" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="17">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="18">
         <v>0.20833333333333301</v>
       </c>
       <c r="C6" s="8">
@@ -2446,10 +2426,10 @@
       <c r="AO6" s="2"/>
     </row>
     <row r="7" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="17">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="18">
         <v>0.25</v>
       </c>
       <c r="C7" s="8">
@@ -2555,10 +2535,10 @@
       <c r="AO7" s="2"/>
     </row>
     <row r="8" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="17">
         <v>0.25</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="18">
         <v>0.29166666666666702</v>
       </c>
       <c r="C8" s="8">
@@ -2664,10 +2644,10 @@
       <c r="AO8" s="2"/>
     </row>
     <row r="9" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="17">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="18">
         <v>0.33333333333333298</v>
       </c>
       <c r="C9" s="8">
@@ -2773,10 +2753,10 @@
       <c r="AO9" s="2"/>
     </row>
     <row r="10" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="17">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="18">
         <v>0.375</v>
       </c>
       <c r="C10" s="8">
@@ -2882,10 +2862,10 @@
       <c r="AO10" s="2"/>
     </row>
     <row r="11" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="17">
         <v>0.375</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="18">
         <v>0.41666666666666702</v>
       </c>
       <c r="C11" s="8">
@@ -2991,10 +2971,10 @@
       <c r="AO11" s="2"/>
     </row>
     <row r="12" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="17">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="18">
         <v>0.45833333333333298</v>
       </c>
       <c r="C12" s="8">
@@ -3100,10 +3080,10 @@
       <c r="AO12" s="2"/>
     </row>
     <row r="13" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="17">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>0.5</v>
       </c>
       <c r="C13" s="8">
@@ -3209,10 +3189,10 @@
       <c r="AO13" s="2"/>
     </row>
     <row r="14" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="17">
         <v>0.5</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="18">
         <v>0.54166666666666696</v>
       </c>
       <c r="C14" s="8">
@@ -3318,10 +3298,10 @@
       <c r="AO14" s="2"/>
     </row>
     <row r="15" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="18">
         <v>0.58333333333333304</v>
       </c>
       <c r="C15" s="8">
@@ -3427,10 +3407,10 @@
       <c r="AO15" s="2"/>
     </row>
     <row r="16" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="17">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="18">
         <v>0.625</v>
       </c>
       <c r="C16" s="8">
@@ -3536,10 +3516,10 @@
       <c r="AO16" s="2"/>
     </row>
     <row r="17" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="17">
         <v>0.625</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>0.66666666666666696</v>
       </c>
       <c r="C17" s="8">
@@ -3645,10 +3625,10 @@
       <c r="AO17" s="2"/>
     </row>
     <row r="18" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="17">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="18">
         <v>0.70833333333333304</v>
       </c>
       <c r="C18" s="8">
@@ -3754,10 +3734,10 @@
       <c r="AO18" s="2"/>
     </row>
     <row r="19" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="17">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>0.75</v>
       </c>
       <c r="C19" s="8">
@@ -3863,10 +3843,10 @@
       <c r="AO19" s="2"/>
     </row>
     <row r="20" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="17">
         <v>0.75</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="18">
         <v>0.79166666666666696</v>
       </c>
       <c r="C20" s="8">
@@ -3972,10 +3952,10 @@
       <c r="AO20" s="2"/>
     </row>
     <row r="21" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="17">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="18">
         <v>0.83333333333333304</v>
       </c>
       <c r="C21" s="8">
@@ -4081,10 +4061,10 @@
       <c r="AO21" s="2"/>
     </row>
     <row r="22" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="17">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="18">
         <v>0.875</v>
       </c>
       <c r="C22" s="8">
@@ -4190,10 +4170,10 @@
       <c r="AO22" s="2"/>
     </row>
     <row r="23" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="A23" s="17">
         <v>0.875</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="18">
         <v>0.91666666666666696</v>
       </c>
       <c r="C23" s="8">
@@ -4299,10 +4279,10 @@
       <c r="AO23" s="2"/>
     </row>
     <row r="24" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="17">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="18">
         <v>0.95833333333333304</v>
       </c>
       <c r="C24" s="8">
@@ -4408,10 +4388,10 @@
       <c r="AO24" s="2"/>
     </row>
     <row r="25" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="17">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8">
@@ -4560,8 +4540,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -4603,8 +4583,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -4646,8 +4626,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -6151,12 +6131,12 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
@@ -6175,8 +6155,8 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6196,10 +6176,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -8962,8 +8944,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -9005,8 +8987,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -9048,8 +9030,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -10553,11 +10535,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -10577,8 +10558,8 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10599,10 +10580,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -13317,8 +13300,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -13360,8 +13343,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -13403,8 +13386,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -14908,11 +14891,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -14932,8 +14914,8 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView topLeftCell="E5" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="AA1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14953,10 +14935,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -17719,8 +17703,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -17762,8 +17746,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -17805,8 +17789,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -19310,11 +19294,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -19334,13 +19317,14 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E36"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AH25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.08984375" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.7265625" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.08984375" style="1" customWidth="1"/>
@@ -19355,11 +19339,13 @@
     <col min="35" max="16384" width="10.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -19460,13 +19446,12 @@
       <c r="AL1" s="2"/>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-    </row>
-    <row r="2" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    </row>
+    <row r="2" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="18">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="C2" s="8">
@@ -19563,13 +19548,12 @@
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-    </row>
-    <row r="3" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    </row>
+    <row r="3" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="18">
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="C3" s="8">
@@ -19666,13 +19650,12 @@
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-    </row>
-    <row r="4" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+    </row>
+    <row r="4" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="18">
         <v>0.125</v>
       </c>
       <c r="C4" s="8">
@@ -19769,13 +19752,12 @@
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-    </row>
-    <row r="5" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+    </row>
+    <row r="5" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>0.125</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="18">
         <v>0.16666666666666699</v>
       </c>
       <c r="C5" s="8">
@@ -19872,13 +19854,12 @@
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
-    </row>
-    <row r="6" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+    </row>
+    <row r="6" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="18">
         <v>0.20833333333333301</v>
       </c>
       <c r="C6" s="8">
@@ -19975,13 +19956,12 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-    </row>
-    <row r="7" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+    </row>
+    <row r="7" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="18">
         <v>0.25</v>
       </c>
       <c r="C7" s="8">
@@ -20078,13 +20058,12 @@
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-    </row>
-    <row r="8" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+    </row>
+    <row r="8" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>0.25</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="18">
         <v>0.29166666666666702</v>
       </c>
       <c r="C8" s="8">
@@ -20181,13 +20160,12 @@
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-    </row>
-    <row r="9" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+    </row>
+    <row r="9" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="18">
         <v>0.33333333333333298</v>
       </c>
       <c r="C9" s="8">
@@ -20284,13 +20262,12 @@
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-    </row>
-    <row r="10" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    </row>
+    <row r="10" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="18">
         <v>0.375</v>
       </c>
       <c r="C10" s="8">
@@ -20387,13 +20364,12 @@
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
-    </row>
-    <row r="11" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+    </row>
+    <row r="11" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>0.375</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="18">
         <v>0.41666666666666702</v>
       </c>
       <c r="C11" s="8">
@@ -20490,13 +20466,12 @@
       <c r="AL11" s="2"/>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-    </row>
-    <row r="12" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+    </row>
+    <row r="12" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="18">
         <v>0.45833333333333298</v>
       </c>
       <c r="C12" s="8">
@@ -20593,13 +20568,12 @@
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
-      <c r="AO12" s="2"/>
-    </row>
-    <row r="13" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+    </row>
+    <row r="13" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>0.5</v>
       </c>
       <c r="C13" s="8">
@@ -20696,13 +20670,12 @@
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-    </row>
-    <row r="14" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+    </row>
+    <row r="14" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
         <v>0.5</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="18">
         <v>0.54166666666666696</v>
       </c>
       <c r="C14" s="8">
@@ -20799,13 +20772,12 @@
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
-    </row>
-    <row r="15" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+    </row>
+    <row r="15" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="18">
         <v>0.58333333333333304</v>
       </c>
       <c r="C15" s="8">
@@ -20902,13 +20874,12 @@
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
-      <c r="AO15" s="2"/>
-    </row>
-    <row r="16" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+    </row>
+    <row r="16" spans="1:40" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="18">
         <v>0.625</v>
       </c>
       <c r="C16" s="8">
@@ -21005,13 +20976,12 @@
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
-      <c r="AO16" s="2"/>
     </row>
     <row r="17" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="17">
         <v>0.625</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>0.66666666666666696</v>
       </c>
       <c r="C17" s="8">
@@ -21108,13 +21078,12 @@
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
-      <c r="AO17" s="2"/>
     </row>
     <row r="18" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="17">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="18">
         <v>0.70833333333333304</v>
       </c>
       <c r="C18" s="8">
@@ -21211,13 +21180,12 @@
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
-      <c r="AO18" s="2"/>
     </row>
     <row r="19" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="17">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>0.75</v>
       </c>
       <c r="C19" s="8">
@@ -21314,13 +21282,12 @@
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
-      <c r="AO19" s="2"/>
     </row>
     <row r="20" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="17">
         <v>0.75</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="18">
         <v>0.79166666666666696</v>
       </c>
       <c r="C20" s="8">
@@ -21417,13 +21384,12 @@
       <c r="AL20" s="2"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
-      <c r="AO20" s="2"/>
     </row>
     <row r="21" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="17">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="18">
         <v>0.83333333333333304</v>
       </c>
       <c r="C21" s="8">
@@ -21520,13 +21486,12 @@
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
-      <c r="AO21" s="2"/>
     </row>
     <row r="22" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="17">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="18">
         <v>0.875</v>
       </c>
       <c r="C22" s="8">
@@ -21623,13 +21588,12 @@
       <c r="AL22" s="2"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
-      <c r="AO22" s="2"/>
     </row>
     <row r="23" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="A23" s="17">
         <v>0.875</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="18">
         <v>0.91666666666666696</v>
       </c>
       <c r="C23" s="8">
@@ -21726,13 +21690,12 @@
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
-      <c r="AO23" s="2"/>
     </row>
     <row r="24" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="17">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="18">
         <v>0.95833333333333304</v>
       </c>
       <c r="C24" s="8">
@@ -21829,13 +21792,12 @@
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
-      <c r="AO24" s="2"/>
     </row>
     <row r="25" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="17">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8">
@@ -21932,12 +21894,9 @@
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
-      <c r="AO25" s="2"/>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -21980,8 +21939,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -22023,8 +21982,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -22066,8 +22025,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -23571,12 +23530,12 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>0</formula>
@@ -23595,13 +23554,14 @@
   </sheetPr>
   <dimension ref="A1:AO65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.08984375" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.7265625" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.08984375" style="1" customWidth="1"/>
@@ -23616,10 +23576,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -23723,10 +23685,10 @@
       <c r="AO1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="18">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="C2" s="8">
@@ -23832,10 +23794,10 @@
       <c r="AO2" s="2"/>
     </row>
     <row r="3" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="17">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="18">
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="C3" s="8">
@@ -23941,10 +23903,10 @@
       <c r="AO3" s="2"/>
     </row>
     <row r="4" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="18">
         <v>0.125</v>
       </c>
       <c r="C4" s="8">
@@ -24050,10 +24012,10 @@
       <c r="AO4" s="2"/>
     </row>
     <row r="5" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="17">
         <v>0.125</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="18">
         <v>0.16666666666666699</v>
       </c>
       <c r="C5" s="8">
@@ -24159,10 +24121,10 @@
       <c r="AO5" s="2"/>
     </row>
     <row r="6" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="17">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="18">
         <v>0.20833333333333301</v>
       </c>
       <c r="C6" s="8">
@@ -24268,10 +24230,10 @@
       <c r="AO6" s="2"/>
     </row>
     <row r="7" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="17">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="18">
         <v>0.25</v>
       </c>
       <c r="C7" s="8">
@@ -24377,10 +24339,10 @@
       <c r="AO7" s="2"/>
     </row>
     <row r="8" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="17">
         <v>0.25</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="18">
         <v>0.29166666666666702</v>
       </c>
       <c r="C8" s="8">
@@ -24486,10 +24448,10 @@
       <c r="AO8" s="2"/>
     </row>
     <row r="9" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="17">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="18">
         <v>0.33333333333333298</v>
       </c>
       <c r="C9" s="8">
@@ -24595,10 +24557,10 @@
       <c r="AO9" s="2"/>
     </row>
     <row r="10" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="17">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="18">
         <v>0.375</v>
       </c>
       <c r="C10" s="8">
@@ -24704,10 +24666,10 @@
       <c r="AO10" s="2"/>
     </row>
     <row r="11" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="17">
         <v>0.375</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="18">
         <v>0.41666666666666702</v>
       </c>
       <c r="C11" s="8">
@@ -24813,10 +24775,10 @@
       <c r="AO11" s="2"/>
     </row>
     <row r="12" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="17">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="18">
         <v>0.45833333333333298</v>
       </c>
       <c r="C12" s="8">
@@ -24922,10 +24884,10 @@
       <c r="AO12" s="2"/>
     </row>
     <row r="13" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="17">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>0.5</v>
       </c>
       <c r="C13" s="8">
@@ -25031,10 +24993,10 @@
       <c r="AO13" s="2"/>
     </row>
     <row r="14" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="17">
         <v>0.5</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="18">
         <v>0.54166666666666696</v>
       </c>
       <c r="C14" s="8">
@@ -25140,10 +25102,10 @@
       <c r="AO14" s="2"/>
     </row>
     <row r="15" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="18">
         <v>0.58333333333333304</v>
       </c>
       <c r="C15" s="8">
@@ -25249,10 +25211,10 @@
       <c r="AO15" s="2"/>
     </row>
     <row r="16" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="17">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="18">
         <v>0.625</v>
       </c>
       <c r="C16" s="8">
@@ -25358,10 +25320,10 @@
       <c r="AO16" s="2"/>
     </row>
     <row r="17" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="17">
         <v>0.625</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>0.66666666666666696</v>
       </c>
       <c r="C17" s="8">
@@ -25467,10 +25429,10 @@
       <c r="AO17" s="2"/>
     </row>
     <row r="18" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="17">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="18">
         <v>0.70833333333333304</v>
       </c>
       <c r="C18" s="8">
@@ -25576,10 +25538,10 @@
       <c r="AO18" s="2"/>
     </row>
     <row r="19" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="17">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>0.75</v>
       </c>
       <c r="C19" s="8">
@@ -25685,10 +25647,10 @@
       <c r="AO19" s="2"/>
     </row>
     <row r="20" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="17">
         <v>0.75</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="18">
         <v>0.79166666666666696</v>
       </c>
       <c r="C20" s="8">
@@ -25794,10 +25756,10 @@
       <c r="AO20" s="2"/>
     </row>
     <row r="21" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="17">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="18">
         <v>0.83333333333333304</v>
       </c>
       <c r="C21" s="8">
@@ -25903,10 +25865,10 @@
       <c r="AO21" s="2"/>
     </row>
     <row r="22" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="17">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="18">
         <v>0.875</v>
       </c>
       <c r="C22" s="8">
@@ -26012,10 +25974,10 @@
       <c r="AO22" s="2"/>
     </row>
     <row r="23" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="A23" s="17">
         <v>0.875</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="18">
         <v>0.91666666666666696</v>
       </c>
       <c r="C23" s="8">
@@ -26121,10 +26083,10 @@
       <c r="AO23" s="2"/>
     </row>
     <row r="24" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="17">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="18">
         <v>0.95833333333333304</v>
       </c>
       <c r="C24" s="8">
@@ -26230,10 +26192,10 @@
       <c r="AO24" s="2"/>
     </row>
     <row r="25" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="17">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8">
@@ -26468,8 +26430,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -26511,8 +26473,8 @@
       <c r="AO29" s="2"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -26554,8 +26516,8 @@
       <c r="AO30" s="2"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -28059,11 +28021,10 @@
       <c r="AO65" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -28083,13 +28044,14 @@
   </sheetPr>
   <dimension ref="A1:AO65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.08984375" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.7265625" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.08984375" style="1" customWidth="1"/>
@@ -28105,10 +28067,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -28212,10 +28176,10 @@
       <c r="AO1" s="2"/>
     </row>
     <row r="2" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="18">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="C2" s="8">
@@ -28319,10 +28283,10 @@
       <c r="AO2" s="2"/>
     </row>
     <row r="3" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="17">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="18">
         <v>8.3333333333333398E-2</v>
       </c>
       <c r="C3" s="8">
@@ -28426,10 +28390,10 @@
       <c r="AO3" s="2"/>
     </row>
     <row r="4" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="17">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="18">
         <v>0.125</v>
       </c>
       <c r="C4" s="8">
@@ -28533,10 +28497,10 @@
       <c r="AO4" s="2"/>
     </row>
     <row r="5" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="17">
         <v>0.125</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="18">
         <v>0.16666666666666699</v>
       </c>
       <c r="C5" s="8">
@@ -28640,10 +28604,10 @@
       <c r="AO5" s="2"/>
     </row>
     <row r="6" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="17">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="18">
         <v>0.20833333333333301</v>
       </c>
       <c r="C6" s="8">
@@ -28747,10 +28711,10 @@
       <c r="AO6" s="2"/>
     </row>
     <row r="7" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="17">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="18">
         <v>0.25</v>
       </c>
       <c r="C7" s="8">
@@ -28854,10 +28818,10 @@
       <c r="AO7" s="2"/>
     </row>
     <row r="8" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="17">
         <v>0.25</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="18">
         <v>0.29166666666666702</v>
       </c>
       <c r="C8" s="8">
@@ -28961,10 +28925,10 @@
       <c r="AO8" s="2"/>
     </row>
     <row r="9" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="17">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="18">
         <v>0.33333333333333298</v>
       </c>
       <c r="C9" s="8">
@@ -29068,10 +29032,10 @@
       <c r="AO9" s="2"/>
     </row>
     <row r="10" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="17">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="18">
         <v>0.375</v>
       </c>
       <c r="C10" s="8">
@@ -29175,10 +29139,10 @@
       <c r="AO10" s="2"/>
     </row>
     <row r="11" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="17">
         <v>0.375</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="18">
         <v>0.41666666666666702</v>
       </c>
       <c r="C11" s="8">
@@ -29282,10 +29246,10 @@
       <c r="AO11" s="2"/>
     </row>
     <row r="12" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="17">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="18">
         <v>0.45833333333333298</v>
       </c>
       <c r="C12" s="8">
@@ -29389,10 +29353,10 @@
       <c r="AO12" s="2"/>
     </row>
     <row r="13" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="17">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>0.5</v>
       </c>
       <c r="C13" s="8">
@@ -29496,10 +29460,10 @@
       <c r="AO13" s="2"/>
     </row>
     <row r="14" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="17">
         <v>0.5</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="18">
         <v>0.54166666666666696</v>
       </c>
       <c r="C14" s="8">
@@ -29603,10 +29567,10 @@
       <c r="AO14" s="2"/>
     </row>
     <row r="15" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="18">
         <v>0.58333333333333304</v>
       </c>
       <c r="C15" s="8">
@@ -29710,10 +29674,10 @@
       <c r="AO15" s="2"/>
     </row>
     <row r="16" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="17">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="18">
         <v>0.625</v>
       </c>
       <c r="C16" s="8">
@@ -29817,10 +29781,10 @@
       <c r="AO16" s="2"/>
     </row>
     <row r="17" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="17">
         <v>0.625</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>0.66666666666666696</v>
       </c>
       <c r="C17" s="8">
@@ -29924,10 +29888,10 @@
       <c r="AO17" s="2"/>
     </row>
     <row r="18" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="17">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="18">
         <v>0.70833333333333304</v>
       </c>
       <c r="C18" s="8">
@@ -30031,10 +29995,10 @@
       <c r="AO18" s="2"/>
     </row>
     <row r="19" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="17">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>0.75</v>
       </c>
       <c r="C19" s="8">
@@ -30138,10 +30102,10 @@
       <c r="AO19" s="2"/>
     </row>
     <row r="20" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="17">
         <v>0.75</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="18">
         <v>0.79166666666666696</v>
       </c>
       <c r="C20" s="8">
@@ -30245,10 +30209,10 @@
       <c r="AO20" s="2"/>
     </row>
     <row r="21" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="17">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="18">
         <v>0.83333333333333304</v>
       </c>
       <c r="C21" s="8">
@@ -30352,10 +30316,10 @@
       <c r="AO21" s="2"/>
     </row>
     <row r="22" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+      <c r="A22" s="17">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="18">
         <v>0.875</v>
       </c>
       <c r="C22" s="8">
@@ -30459,10 +30423,10 @@
       <c r="AO22" s="2"/>
     </row>
     <row r="23" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+      <c r="A23" s="17">
         <v>0.875</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="18">
         <v>0.91666666666666696</v>
       </c>
       <c r="C23" s="8">
@@ -30566,10 +30530,10 @@
       <c r="AO23" s="2"/>
     </row>
     <row r="24" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="17">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="18">
         <v>0.95833333333333304</v>
       </c>
       <c r="C24" s="8">
@@ -30673,10 +30637,10 @@
       <c r="AO24" s="2"/>
     </row>
     <row r="25" spans="1:41" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="17">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8">
@@ -30909,8 +30873,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -30952,8 +30916,8 @@
       <c r="AO29" s="2"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -30995,8 +30959,8 @@
       <c r="AO30" s="2"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -32500,11 +32464,10 @@
       <c r="AO65" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -32524,8 +32487,8 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -32545,10 +32508,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -35311,8 +35276,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -35354,8 +35319,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -35397,8 +35362,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -36902,11 +36867,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -36926,13 +36890,14 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" customWidth="1"/>
     <col min="3" max="6" width="10.08984375" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.7265625" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.08984375" style="1" customWidth="1"/>
@@ -36948,10 +36913,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -39519,8 +39486,8 @@
       <c r="A25" s="10">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>0</v>
+      <c r="B25" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="C25" s="8">
         <v>138.64032692999999</v>
@@ -39666,8 +39633,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -39709,8 +39676,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -39752,8 +39719,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -41257,11 +41224,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -41282,7 +41248,7 @@
   <dimension ref="A1:AO63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -41302,10 +41268,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -44068,8 +44036,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -44111,8 +44079,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -44154,8 +44122,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -45659,11 +45627,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -45683,8 +45650,8 @@
   </sheetPr>
   <dimension ref="A1:AO63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -45704,10 +45671,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -48470,8 +48439,8 @@
       <c r="AO26" s="2"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -48513,8 +48482,8 @@
       <c r="AO27" s="2"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -48556,8 +48525,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -50061,11 +50030,10 @@
       <c r="AO63" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
@@ -50085,8 +50053,8 @@
   </sheetPr>
   <dimension ref="A1:AO65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" activeCellId="1" sqref="A1:XFD1 A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -50107,10 +50075,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="12">
         <v>1</v>
       </c>
@@ -52911,8 +52881,8 @@
       <c r="AO28" s="2"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -52954,8 +52924,8 @@
       <c r="AO29" s="2"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -52997,8 +52967,8 @@
       <c r="AO30" s="2"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -54502,11 +54472,10 @@
       <c r="AO65" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:AG25">
     <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThanOrEqual">

</xml_diff>